<commit_message>
extended dummy data - added propensity covariate table
</commit_message>
<xml_diff>
--- a/1_data/Opal_dummy_data.xlsx
+++ b/1_data/Opal_dummy_data.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanjinli/Desktop/McGill 2021/PPHS 630 Practicum/opal-assessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/opal-assessment/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20E2D8C-9158-0940-9BAE-FAE9E0E61BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{E20E2D8C-9158-0940-9BAE-FAE9E0E61BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BBB4A0D-BB61-5D43-9E28-E5916CE754D4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{C8F546A3-2F7B-8C4A-A9B1-A0E7B0FAE806}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{C8F546A3-2F7B-8C4A-A9B1-A0E7B0FAE806}"/>
   </bookViews>
   <sheets>
     <sheet name="visit_data" sheetId="1" r:id="rId1"/>
     <sheet name="opal_usr_list" sheetId="2" r:id="rId2"/>
+    <sheet name="propens_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">visit_data!$A$1:$E$390</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +88,39 @@
   </si>
   <si>
     <t>ep_end</t>
+  </si>
+  <si>
+    <t>pastyear_ED_visits</t>
+  </si>
+  <si>
+    <t>past_year_hospitalization</t>
+  </si>
+  <si>
+    <t>prior_cancer</t>
+  </si>
+  <si>
+    <t>cancer_stage</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>prefered_language</t>
+  </si>
+  <si>
+    <t>cancer_site</t>
+  </si>
+  <si>
+    <t>login2</t>
+  </si>
+  <si>
+    <t>login3</t>
+  </si>
+  <si>
+    <t>login4</t>
   </si>
 </sst>
 </file>
@@ -441,9 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C8E4E8-E3C9-004D-A9BF-A42F6EC9AB08}">
   <dimension ref="A1:K390"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7112,23 +7144,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87E7060-9C9E-DC49-AEF0-A142E5683001}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7136,7 +7177,7 @@
         <v>44064</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -7144,7 +7185,7 @@
         <v>43930</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -7152,7 +7193,7 @@
         <v>43946</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
@@ -7160,7 +7201,7 @@
         <v>44151</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>10</v>
       </c>
@@ -7168,7 +7209,7 @@
         <v>43793</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
@@ -7176,7 +7217,7 @@
         <v>43926</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
@@ -7184,7 +7225,7 @@
         <v>44074</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>17</v>
       </c>
@@ -7192,7 +7233,7 @@
         <v>44156</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>22</v>
       </c>
@@ -7200,7 +7241,7 @@
         <v>43813</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>24</v>
       </c>
@@ -7208,12 +7249,191 @@
         <v>43836</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>43560</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA65AF5-B72A-FC49-AA8A-4E807F767A43}">
+  <dimension ref="A1:I26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add multiple login times for each patient
</commit_message>
<xml_diff>
--- a/1_data/Opal_dummy_data.xlsx
+++ b/1_data/Opal_dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanjinli/Desktop/McGill 2021/PPHS 630 Practicum/opal-assessment/1_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B096B63-40A3-B344-A48C-71A49CD633F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6124B9-3B11-114F-A617-F5965364E9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{C8F546A3-2F7B-8C4A-A9B1-A0E7B0FAE806}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -69,27 +69,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>First_login</t>
-  </si>
-  <si>
-    <t>last_visit_date</t>
-  </si>
-  <si>
-    <t>next_visit_date</t>
-  </si>
-  <si>
-    <t>days_next</t>
-  </si>
-  <si>
-    <t>days_last</t>
-  </si>
-  <si>
-    <t>ep_start</t>
-  </si>
-  <si>
-    <t>ep_end</t>
-  </si>
-  <si>
     <t>pastyear_ED_visits</t>
   </si>
   <si>
@@ -114,13 +93,7 @@
     <t>cancer_site</t>
   </si>
   <si>
-    <t>login2</t>
-  </si>
-  <si>
-    <t>login3</t>
-  </si>
-  <si>
-    <t>login4</t>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -473,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C8E4E8-E3C9-004D-A9BF-A42F6EC9AB08}">
-  <dimension ref="A1:K390"/>
+  <dimension ref="A1:E390"/>
   <sheetViews>
-    <sheetView topLeftCell="A367" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +459,7 @@
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -502,26 +475,8 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -538,7 +493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -555,7 +510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -572,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -589,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -606,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -623,7 +578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -640,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -657,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -674,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -691,7 +646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -708,7 +663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -725,7 +680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -742,7 +697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -759,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -7146,10 +7101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87E7060-9C9E-DC49-AEF0-A142E5683001}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7159,16 +7114,7 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7178,183 +7124,471 @@
       <c r="B2" s="1">
         <v>44064</v>
       </c>
-      <c r="C2" s="1">
-        <v>44273</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44288</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44370</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>43930</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44094</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44101</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44206</v>
-      </c>
+        <v>44273</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>43946</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44411</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44497</v>
-      </c>
-      <c r="E4" s="1">
-        <v>44497</v>
-      </c>
+        <v>44288</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>44151</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44407</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44473</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44511</v>
-      </c>
+        <v>44370</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>43793</v>
-      </c>
-      <c r="C6" s="1">
-        <v>44412</v>
-      </c>
-      <c r="D6" s="1">
-        <v>44512</v>
-      </c>
-      <c r="E6" s="1">
-        <v>44529</v>
-      </c>
+        <v>43930</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>43926</v>
-      </c>
-      <c r="C7" s="1">
-        <v>44051</v>
-      </c>
-      <c r="D7" s="1">
-        <v>44529</v>
-      </c>
-      <c r="E7" s="1">
-        <v>44538</v>
-      </c>
+        <v>44094</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>44074</v>
-      </c>
-      <c r="C8" s="1">
-        <v>44092</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44215</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44350</v>
-      </c>
+        <v>44101</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>44156</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44320</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44509</v>
-      </c>
-      <c r="E9" s="1">
-        <v>44540</v>
-      </c>
+        <v>44206</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
-        <v>43813</v>
-      </c>
-      <c r="C10" s="1">
-        <v>44216</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44466</v>
-      </c>
-      <c r="E10" s="1">
-        <v>44499</v>
-      </c>
+        <v>43946</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
-        <v>43836</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44140</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44238</v>
-      </c>
-      <c r="E11" s="1">
-        <v>44249</v>
-      </c>
+        <v>44411</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44489</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44497</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44151</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44407</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44473</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44511</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43793</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44412</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44512</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44529</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>43926</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44051</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44529</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44538</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44074</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44092</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44215</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44350</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44156</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44320</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>17</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44509</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44540</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43813</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44216</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44466</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>22</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44499</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>24</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43836</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>24</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44140</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44238</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44249</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>25</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B42" s="1">
         <v>43560</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>25</v>
+      </c>
+      <c r="B43" s="1">
         <v>44094</v>
       </c>
-      <c r="D12" s="1">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44" s="1">
         <v>44228</v>
       </c>
-      <c r="E12" s="1">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>25</v>
+      </c>
+      <c r="B45" s="1">
         <v>44272</v>
       </c>
     </row>
@@ -7389,28 +7623,28 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>